<commit_message>
rename, delete and update 2025-06-26
</commit_message>
<xml_diff>
--- a/Investing ben natan shulman.xlsx
+++ b/Investing ben natan shulman.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1069c69fb87cd973/Finencial/repo_investing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1069C69FB87CD973/Finencial/repo_investing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5521" documentId="13_ncr:1_{6684F656-A1AF-432B-BD61-498F4564DF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB7D2D20-09C2-4D72-BDF0-0FE1D84D4D18}"/>
+  <xr:revisionPtr revIDLastSave="6074" documentId="13_ncr:1_{6684F656-A1AF-432B-BD61-498F4564DF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EF3A8D1-2533-4213-854D-8B0A7DEDE5FC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C236A5B8-795C-467A-8F0F-269E9F656624}"/>
+    <workbookView xWindow="8055" yWindow="2505" windowWidth="28800" windowHeight="15345" xr2:uid="{C236A5B8-795C-467A-8F0F-269E9F656624}"/>
   </bookViews>
   <sheets>
     <sheet name="Yigael Isreal" sheetId="2" r:id="rId1"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
   <si>
     <t>Instrument</t>
   </si>
@@ -609,6 +609,9 @@
   <si>
     <t>טאואר</t>
   </si>
+  <si>
+    <t>דניה סיבוס</t>
+  </si>
 </sst>
 </file>
 
@@ -620,7 +623,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,6 +684,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222020"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -722,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -746,6 +755,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,10 +1005,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -1128,9 +1134,9 @@
     <v>4</v>
     <v>72.83</v>
     <v>39.97</v>
-    <v>0.98060000000000003</v>
-    <v>-0.49</v>
-    <v>-9.0720000000000002E-3</v>
+    <v>0.96440000000000003</v>
+    <v>0.75</v>
+    <v>1.4657E-2</v>
     <v>USD</v>
     <v>Exact Sciences Corporation is a provider of cancer screening and diagnostic tests. The Company provides a portfolio of products for earlier cancer detection and treatment guidance. Its products and services focus on screening and precision oncology tests. It is focusing its research and development efforts on three main areas: Colorectal Cancer Screening Test Development, MCED Test Development and MRD Test Development. Its products and services include Cologuard test, Oncotype DX Breast Recurrence Score Test, Oncotype DX Breast DCIS Score Test, Oncotype DX Colon Recurrence Score Test, OncoExTra Test, and Riskguard Test. Its flagship screening product, the Cologuard test, is a non-invasive, stool-based deoxyribonucleic acid (sDNA) screening test that utilizes a multi-target approach to detect DNA and hemoglobin biomarkers associated with colorectal cancer and pre-cancer. The Oncotype DX Breast Recurrence Score test examines the activity of 21 genes in a patient’s breast tumor tissue.</v>
     <v>6900</v>
@@ -1138,24 +1144,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>5505 Endeavor Lane, MADISON, WI, 53719 US</v>
-    <v>54.21</v>
+    <v>52.16</v>
     <v>Biotechnology &amp; Medical Research</v>
     <v>Stock</v>
-    <v>45821.976476978904</v>
+    <v>45833.999552025001</v>
     <v>0</v>
-    <v>53.08</v>
-    <v>10095890000</v>
+    <v>50.09</v>
+    <v>9794069384</v>
     <v>EXACT SCIENCES CORPORATION</v>
     <v>EXACT SCIENCES CORPORATION</v>
-    <v>53.2</v>
+    <v>50.93</v>
     <v>0</v>
-    <v>54.01</v>
-    <v>53.52</v>
+    <v>51.17</v>
+    <v>51.92</v>
     <v>188637700</v>
     <v>EXAS</v>
     <v>EXACT SCIENCES CORPORATION (XNAS:EXAS)</v>
-    <v>1266219</v>
-    <v>3010147</v>
+    <v>54</v>
+    <v>2943361</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -1176,12 +1182,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>153.13</v>
+    <v>5</v>
+    <v>154.44999999999999</v>
     <v>86.62</v>
-    <v>2.1208999999999998</v>
-    <v>-3.03</v>
-    <v>-2.0897000000000002E-2</v>
+    <v>2.1206999999999998</v>
+    <v>6.41</v>
+    <v>4.3339999999999997E-2</v>
     <v>USD</v>
     <v>NVIDIA Corporation is a full-stack computing infrastructure company. The Company is engaged in accelerated computing to help solve the challenging computational problems. The Company’s segments include Compute &amp; Networking and Graphics. The Compute &amp; Networking segment includes its Data Center accelerated computing platforms and artificial intelligence (AI) solutions and software; networking; automotive platforms and autonomous and electric vehicle solutions; Jetson for robotics and other embedded platforms, and DGX Cloud computing services. The Graphics segment includes GeForce GPUs for gaming and PCs, the GeForce NOW game streaming service and related infrastructure, and solutions for gaming platforms; Quadro/NVIDIA RTX GPUs for enterprise workstation graphics; virtual GPU software for cloud-based visual and virtual computing; automotive platforms for infotainment systems, and Omniverse Enterprise software for building and operating industrial AI and digital twin applications.</v>
     <v>36000</v>
@@ -1189,24 +1195,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>2788 San Tomas Expressway, SANTA CLARA, CA, 95051 US</v>
-    <v>143.58000000000001</v>
+    <v>154.44999999999999</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.999999305466</v>
+    <v>45833.999984282033</v>
     <v>3</v>
-    <v>140.85499999999999</v>
-    <v>3464068000000</v>
+    <v>149.26</v>
+    <v>3765164000000</v>
     <v>NVIDIA CORPORATION</v>
     <v>NVIDIA CORPORATION</v>
-    <v>142.47999999999999</v>
-    <v>45.730499999999999</v>
-    <v>145</v>
-    <v>141.97</v>
+    <v>149.27000000000001</v>
+    <v>49.705399999999997</v>
+    <v>147.9</v>
+    <v>154.31</v>
     <v>24400000000</v>
     <v>NVDA</v>
     <v>NVIDIA CORPORATION (XNAS:NVDA)</v>
-    <v>194269</v>
-    <v>219249131</v>
+    <v>1981347</v>
+    <v>204376250</v>
     <v>1998</v>
   </rv>
   <rv s="2">
@@ -1230,9 +1236,9 @@
     <v>5</v>
     <v>64.05</v>
     <v>34.590000000000003</v>
-    <v>2.3483999999999998</v>
-    <v>-3.47</v>
-    <v>-6.2264E-2</v>
+    <v>2.3105000000000002</v>
+    <v>-0.98</v>
+    <v>-1.8681E-2</v>
     <v>USD</v>
     <v>On Holding AG is a Switzerland-based company active in athletic sports accesories industry. The Company provides footwear and sports apparel and is engaged in developing and distributing performance sports products, through independent retailers and global distributors. The Company sells its products trough the internet and its own stores.</v>
     <v>3254</v>
@@ -1240,24 +1246,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Forrlibuckstrasse 190, ZUERICH, ZUERICH, 8005 CH</v>
-    <v>55.45</v>
+    <v>52.99</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45821.997693888283</v>
+    <v>45833.999649814061</v>
     <v>6</v>
-    <v>51.12</v>
-    <v>17043270000</v>
+    <v>51</v>
+    <v>16788894407</v>
     <v>On Holding Ltd</v>
     <v>On Holding Ltd</v>
-    <v>54.24</v>
-    <v>73.413899999999998</v>
-    <v>55.73</v>
-    <v>52.26</v>
+    <v>52.89</v>
+    <v>72.318200000000004</v>
+    <v>52.46</v>
+    <v>51.48</v>
     <v>326124600</v>
     <v>ONON</v>
     <v>On Holding Ltd (XNYS:ONON)</v>
-    <v>649</v>
-    <v>5057875</v>
+    <v>444</v>
+    <v>4140483</v>
     <v>2012</v>
   </rv>
   <rv s="2">
@@ -1278,12 +1284,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>55.31</v>
     <v>28.64</v>
-    <v>0.77749999999999997</v>
-    <v>-2.13</v>
-    <v>-5.2958999999999999E-2</v>
+    <v>0.78410000000000002</v>
+    <v>0.19</v>
+    <v>4.4549999999999998E-3</v>
     <v>USD</v>
     <v>Tower Semiconductor Ltd. operates as an independent semiconductor foundry focused primarily on specialty process technologies. The Company focuses on producing integrated circuits (ICs) based on the design specifications of its customers. The Company manufactures semiconductors for its customers primarily based on third-party designs. It offers process manufacture geometries of 0.35, 0.50, 0.55, 0.60, 0.80-micron and above on 150 millimeter wafers, 0.35, 0.18. 0.16, 0.13 and 0.11-micron on 200 millimeter wafers, and 65 nanometer and 45 nanometer on 300 millimeter wafers. It also provides design support and technical services. The Company's ICs are incorporated into a range of products in markets, including consumer electronics, personal computers, communications, automotive, industrial and medical device products. The Company has manufacturing facilities in the United States, Israel and Japan.</v>
     <v>5215</v>
@@ -1291,24 +1297,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>20 Shaul Amor Avenue, Ramat Gavriel Industrial Park, Po Box 619, MIGDAL HAEMEQ, 2310502 IL</v>
-    <v>39.659999999999997</v>
+    <v>43.63</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.949278714841</v>
+    <v>45833.985559455468</v>
     <v>9</v>
-    <v>37.479999999999997</v>
-    <v>4260198000</v>
+    <v>42.75</v>
+    <v>4791465504</v>
     <v>TOWER SEMICONDUCTOR LTD</v>
     <v>TOWER SEMICONDUCTOR LTD</v>
-    <v>39.49</v>
-    <v>21.090900000000001</v>
-    <v>40.22</v>
-    <v>38.090000000000003</v>
+    <v>43.42</v>
+    <v>23.7211</v>
+    <v>42.65</v>
+    <v>42.84</v>
     <v>111845600</v>
     <v>TSEM</v>
     <v>TOWER SEMICONDUCTOR LTD (XNAS:TSEM)</v>
-    <v>2623</v>
-    <v>495494</v>
+    <v>534</v>
+    <v>508450</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -1329,12 +1335,12 @@
     <v>2</v>
     <v>7</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>98.15</v>
-    <v>34.409999999999997</v>
-    <v>1.5649999999999999</v>
-    <v>2.06</v>
-    <v>2.1659000000000001E-2</v>
+    <v>5</v>
+    <v>105.3</v>
+    <v>35.270000000000003</v>
+    <v>1.5923</v>
+    <v>-1.94</v>
+    <v>-1.8515E-2</v>
     <v>USD</v>
     <v>Roblox Corporation operates a platform for connection and communication (Roblox Platform), where every day, people come to create, play, work, learn, and connect with each other in experiences built by its global community of creators. The Company’s platform consists of the Roblox Client, the Roblox Studio, and the Roblox Cloud. Roblox Client is an application that allows users to seamlessly explore 3D immersive experiences. Roblox Studio is the free toolset that allows developers and creators to build, publish, and operate three-dimensional (3D) immersive experiences and other content accessed with the Roblox Client. Roblox Cloud includes the services and infrastructure that power its Platform. The Company operates the Roblox Platform as a live service that allows users to play and socialize with others for free. The Company offers developers and creators the ability to build engaging, immersive experiences and marketplace items that they can easily share with the Roblox community.</v>
     <v>2474</v>
@@ -1342,23 +1348,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3150 South Delaware Street, SAN MATEO, CA, 94403 US</v>
-    <v>97.58</v>
+    <v>105.3</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999782500003</v>
+    <v>45833.999704409376</v>
     <v>12</v>
-    <v>93.73</v>
-    <v>65908890000</v>
+    <v>102.735</v>
+    <v>69754757412</v>
     <v>ROBLOX CORPORATION</v>
     <v>ROBLOX CORPORATION</v>
-    <v>93.8</v>
-    <v>95.11</v>
-    <v>97.17</v>
+    <v>104.99</v>
+    <v>104.78</v>
+    <v>102.84</v>
     <v>678284300</v>
     <v>RBLX</v>
     <v>ROBLOX CORPORATION (XNYS:RBLX)</v>
-    <v>2721</v>
-    <v>8686389</v>
+    <v>6861</v>
+    <v>8395291</v>
     <v>2004</v>
   </rv>
   <rv s="2">
@@ -1379,12 +1385,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>140</v>
+    <v>5</v>
+    <v>147.66999999999999</v>
     <v>21.23</v>
-    <v>2.6387</v>
-    <v>2.21</v>
-    <v>1.6347E-2</v>
+    <v>2.6315</v>
+    <v>-0.33</v>
+    <v>-2.3040000000000001E-3</v>
     <v>USD</v>
     <v>Palantir Technologies Inc. is engaged in building software to assist in counterterrorism investigations and operations. The Company has built four principal software platforms, including Palantir Gotham (Gotham), Palantir Foundry (Foundry), Palantir Apollo (Apollo), and Palantir Artificial Intelligence Platform (AIP). Apollo is a cloud-agnostic, single control layer that coordinates ongoing delivery of new features, security updates, and platform configurations, helping to ensure the continuous operation of critical systems. Gotham enables users to identify patterns hidden deep within datasets, ranging from signals intelligence sources to reports from confidential informants. Foundry transforms the ways organizations operate by creating a central operating system for their data. AIP enables responsible artificial intelligence (AI)-advantage across the enterprise by using primary, core components built to effectively activate large language models and other AI within any organization.</v>
     <v>4001</v>
@@ -1392,24 +1398,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1200 17Th Street, Floor 15, DENVER, CO, 80202 US</v>
-    <v>139.99</v>
+    <v>147.66999999999999</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999942881252</v>
+    <v>45833.999977985935</v>
     <v>15</v>
-    <v>133.35</v>
-    <v>324252000000</v>
+    <v>141.53</v>
+    <v>337231424800</v>
     <v>PALANTIR TECHNOLOGIES INC.</v>
     <v>PALANTIR TECHNOLOGIES INC.</v>
-    <v>133.815</v>
-    <v>600.02620000000002</v>
-    <v>135.19</v>
-    <v>137.4</v>
+    <v>144.49</v>
+    <v>624.04470000000003</v>
+    <v>143.22999999999999</v>
+    <v>142.9</v>
     <v>2359912000</v>
     <v>PLTR</v>
     <v>PALANTIR TECHNOLOGIES INC. (XNAS:PLTR)</v>
-    <v>216583</v>
-    <v>89105409</v>
+    <v>178281</v>
+    <v>82972534</v>
     <v>2003</v>
   </rv>
   <rv s="2">
@@ -1430,12 +1436,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>488.53989999999999</v>
-    <v>177</v>
-    <v>2.4613</v>
-    <v>6.2</v>
-    <v>1.9429000000000002E-2</v>
+    <v>182</v>
+    <v>2.4451000000000001</v>
+    <v>-12.92</v>
+    <v>-3.7948000000000003E-2</v>
     <v>USD</v>
     <v>Tesla, Inc. designs, develops, manufactures, sells and leases high-performance fully electric vehicles and energy generation and storage systems, and offers services related to its products. Its segments include automotive, and energy generation and storage. The automotive segment includes the design, development, manufacturing, sales and leasing of high-performance fully electric vehicles, and sales of automotive regulatory credits. It also includes sales of used vehicles, non-warranty maintenance services and collisions, part sales, paid supercharging, insurance services revenue and retail merchandise sales. The energy generation and storage segment include the design, manufacture, installation, sales and leasing of solar energy generation and energy storage products and related services and sales of solar energy systems incentives. Its consumer vehicles include the Model 3, Y, S, X and Cybertruck. Its lithium-ion battery energy storage products include Powerwall and Megapack.</v>
     <v>125665</v>
@@ -1443,24 +1449,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1 Tesla Road, AUSTIN, TX, 78725 US</v>
-    <v>332.99</v>
+    <v>343</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45821.999993564059</v>
+    <v>45833.999998899999</v>
     <v>18</v>
-    <v>313.3</v>
-    <v>1047809000000</v>
+    <v>320.39999999999998</v>
+    <v>1055024137800</v>
     <v>TESLA, INC.</v>
     <v>TESLA, INC.</v>
-    <v>313.97000000000003</v>
-    <v>179.0497</v>
-    <v>319.11</v>
-    <v>325.31</v>
+    <v>342.7</v>
+    <v>180.2826</v>
+    <v>340.47</v>
+    <v>327.55</v>
     <v>3220956000</v>
     <v>TSLA</v>
     <v>TESLA, INC. (XNAS:TSLA)</v>
-    <v>308800</v>
-    <v>119855317</v>
+    <v>821727</v>
+    <v>119852498</v>
     <v>2024</v>
   </rv>
   <rv s="2">
@@ -1481,12 +1487,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>37.159999999999997</v>
     <v>17.664999999999999</v>
-    <v>1.1123000000000001</v>
-    <v>-0.63</v>
-    <v>-3.0331999999999998E-2</v>
+    <v>1.133</v>
+    <v>-0.35</v>
+    <v>-1.5521E-2</v>
     <v>USD</v>
     <v>Intel Corporation is a global designer and manufacturer of semiconductor products. The Company operates through three segments: Intel Products, Intel Foundry, and All Other. Its Intel Products segment includes Client Computing Group (CCG), Data Center and AI (DCAI), Network and Edge (NEX). The CCG is bringing together the operating system, system architecture, hardware, and software application integration to enable PC experiences. DCAI delivers workload-optimized solutions to cloud service providers and enterprises, along with silicon devices for communications service providers, network and edge, and HPC customers. NEX helps networks and edge compute systems from fixed-function hardware to general-purpose compute, acceleration, and networking devices running cloud native software on programmable hardware. The Intel Foundry segment comprises technology development, manufacturing and foundry services. All Other segments include Altera, Mobileye, Other.</v>
     <v>108900</v>
@@ -1494,24 +1500,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>2200 Mission College Blvd, Rnb-4-151, SANTA CLARA, CA, 95054 US</v>
-    <v>20.6</v>
+    <v>22.77</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.999899571092</v>
+    <v>45833.999934467189</v>
     <v>21</v>
-    <v>20.100000000000001</v>
-    <v>87850680000</v>
+    <v>22.125</v>
+    <v>96836400000</v>
     <v>INTEL CORPORATION</v>
     <v>INTEL CORPORATION</v>
-    <v>20.329999999999998</v>
+    <v>22.574999999999999</v>
     <v>0</v>
-    <v>20.77</v>
-    <v>20.14</v>
+    <v>22.55</v>
+    <v>22.2</v>
     <v>4362000000</v>
     <v>INTC</v>
     <v>INTEL CORPORATION (XNAS:INTC)</v>
-    <v>78944</v>
-    <v>78268049</v>
+    <v>194085</v>
+    <v>85967310</v>
     <v>1989</v>
   </rv>
   <rv s="2">
@@ -1532,12 +1538,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>187.28</v>
     <v>76.48</v>
-    <v>1.9927999999999999</v>
-    <v>-2.34</v>
-    <v>-1.9747000000000001E-2</v>
+    <v>2.0196000000000001</v>
+    <v>4.97</v>
+    <v>3.5902999999999997E-2</v>
     <v>USD</v>
     <v>Advanced Micro Devices, Inc. is a global semiconductor company. It is focused on high-performance computing, graphics and visualization technologies. It operates in four segments. The Data Center segment includes artificial intelligence (AI) accelerators, server central processing units (CPUs), graphics processing units (GPUs), accelerated processing units (APUs), data processing units (DPUs), field programmable gate arrays (FPGAs), smart network interface cards (SmartNICs), and Adaptive system-on-chip (SoC) products for data centers. The Client segment primarily includes CPUs, APUs, and chipsets for desktops and notebooks. The Gaming segment primarily includes discrete GPUs, semi-custom SoC products and development services. The Embedded segment includes embedded CPUs, GPUs, APUs, FPGAs, system on modules (SOMs), and Adaptive SoC products. It markets and sells its products under the AMD trademark. Its products include AMD EPYC, AMD Ryzen, AMD Ryzen PRO, Virtex UltraScale+ and others.</v>
     <v>28000</v>
@@ -1545,24 +1551,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>2485 Augustine Drive, SANTA CLARA, CA, 95054 US</v>
-    <v>117.883</v>
+    <v>144.18</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.99997038125</v>
+    <v>45833.999973923441</v>
     <v>24</v>
-    <v>115.06</v>
-    <v>188342300000</v>
+    <v>139.46</v>
+    <v>232509333600</v>
     <v>ADVANCED MICRO DEVICES, INC.</v>
     <v>ADVANCED MICRO DEVICES, INC.</v>
-    <v>116.045</v>
-    <v>85.150700000000001</v>
-    <v>118.5</v>
-    <v>116.16</v>
+    <v>140.94</v>
+    <v>105.1189</v>
+    <v>138.43</v>
+    <v>143.4</v>
     <v>1621404000</v>
     <v>AMD</v>
     <v>ADVANCED MICRO DEVICES, INC. (XNAS:AMD)</v>
-    <v>37030</v>
-    <v>40250246</v>
+    <v>546880</v>
+    <v>45627563</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -1583,12 +1589,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>226.4</v>
     <v>133.57</v>
-    <v>1.27</v>
-    <v>-4.33</v>
-    <v>-2.0098999999999999E-2</v>
+    <v>1.2829999999999999</v>
+    <v>2.65</v>
+    <v>1.2041E-2</v>
     <v>USD</v>
     <v>Taiwan Semiconductor Manufacturing Co Ltd is a Taiwan-based company mainly engaged in the provision of integrated circuit manufacturing services. The integrated circuit manufacturing services include process technology, special process technology, design ecosystem support, mask technology, 3DFabricTM advanced packaging and silicon stacking technology services. The Company has completed the transfer and mass production of 5nm technology, and is engaged in the research and development of 3nm process technology and 2nm process technology. The product application range covers the entire electronic application industry, including personal computers and peripheral products, information application products, wired and wireless communication system products, servers and data centers.</v>
     <v>52045</v>
@@ -1596,24 +1602,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>No.8, Li-Hsin 6th Road, Hsinchu Science Park, HSINCHU, HSINCHU, 300 TW</v>
-    <v>213.26</v>
+    <v>223.5</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.999908818747</v>
+    <v>45833.999981087502</v>
     <v>27</v>
-    <v>209.4</v>
-    <v>905566600000</v>
+    <v>220.8</v>
+    <v>919596300000</v>
     <v>Taiwan Semiconductor Manufacturing Co., Ltd.</v>
     <v>Taiwan Semiconductor Manufacturing Co., Ltd.</v>
-    <v>210.11</v>
-    <v>27.8017</v>
-    <v>215.43</v>
-    <v>211.1</v>
+    <v>220.8</v>
+    <v>29.334599999999998</v>
+    <v>220.09</v>
+    <v>222.74</v>
     <v>5186523000</v>
     <v>TSM</v>
     <v>Taiwan Semiconductor Manufacturing Co., Ltd. (XNYS:TSM)</v>
-    <v>8319</v>
-    <v>11943391</v>
+    <v>39118</v>
+    <v>11144005</v>
     <v>1987</v>
   </rv>
   <rv s="2">
@@ -1634,12 +1640,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>101.402</v>
+    <v>5</v>
+    <v>96.33</v>
     <v>17.25</v>
-    <v>1.3967000000000001</v>
-    <v>-1.8</v>
-    <v>-4.1513000000000001E-2</v>
+    <v>1.3928</v>
+    <v>3.77</v>
+    <v>8.8001999999999997E-2</v>
     <v>USD</v>
     <v>Super Micro Computer, Inc. provides application-optimized Total IT solutions. It delivers rack-scale solutions optimized for various workloads, including artificial intelligence and high-performance computing, where acceleration is critical. It produces a portfolio of server and storage solutions for enterprise data centers, cloud service providers and edge computing (5G Telco, Retail and embedded). Total IT Solutions include complete servers, storage systems, modular blade servers, workstations, full-rack scale solutions, networking devices, server sub-systems, server management and security software. It provides global support and services to help its customers install, upgrade and maintain their computing infrastructure, including liquid-cooling operations. It offers platforms in rackmount, blade, multi-node and embedded form factors, which support single, dual and multiprocessor architectures. Its key product lines include SuperBlade and MicroBlade, SuperStorage, Twin and others.</v>
     <v>5684</v>
@@ -1647,24 +1653,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>980 Rock Avenue, SAN JOSE, CA, 95131 US</v>
-    <v>42.469900000000003</v>
+    <v>46.93</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45821.999957499997</v>
+    <v>45833.999930404687</v>
     <v>30</v>
-    <v>40.744999999999997</v>
-    <v>24803740000</v>
+    <v>43.12</v>
+    <v>27817668336</v>
     <v>SUPER MICRO COMPUTER, INC.</v>
     <v>SUPER MICRO COMPUTER, INC.</v>
-    <v>42.03</v>
-    <v>23.013100000000001</v>
-    <v>43.36</v>
-    <v>41.56</v>
+    <v>43.34</v>
+    <v>25.8094</v>
+    <v>42.84</v>
+    <v>46.61</v>
     <v>596817600</v>
     <v>SMCI</v>
     <v>SUPER MICRO COMPUTER, INC. (XNAS:SMCI)</v>
-    <v>53946</v>
-    <v>48524166</v>
+    <v>284137</v>
+    <v>37838884</v>
     <v>2006</v>
   </rv>
   <rv s="2">
@@ -1683,19 +1689,19 @@
     <v>Finance</v>
     <v>11</v>
     <v>3.8532999999999999</v>
-    <v>3.4651000000000001</v>
-    <v>-7.0900000000000005E-2</v>
-    <v>-1.9601999999999998E-2</v>
+    <v>3.3711000000000002</v>
+    <v>2.3E-3</v>
+    <v>6.7759999999999999E-4</v>
     <v>ILS</v>
     <v>USD</v>
-    <v>3.5968</v>
+    <v>3.4075000000000002</v>
     <v>Currency Pair</v>
-    <v>45824.351921296293</v>
-    <v>3.5428999999999999</v>
+    <v>45834.444027777776</v>
+    <v>3.3711000000000002</v>
     <v>US Dollar/Israeli Shekel FX Spot Rate</v>
-    <v>3.5819000000000001</v>
-    <v>3.617</v>
-    <v>3.5461</v>
+    <v>3.3963000000000001</v>
+    <v>3.3942999999999999</v>
+    <v>3.3965999999999998</v>
     <v>USDILS</v>
     <v>USD/ILS</v>
   </rv>
@@ -1717,12 +1723,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>24.98</v>
     <v>3.82</v>
-    <v>1.6379999999999999</v>
-    <v>-0.37</v>
-    <v>-3.9070999999999995E-2</v>
+    <v>1.78</v>
+    <v>-0.25</v>
+    <v>-2.5457999999999998E-2</v>
     <v>USD</v>
     <v>SoundHound AI, Inc. is engaged in conversational intelligence, offering voice and conversational artificial intelligence (AI) solutions that let businesses offer experiences to their customers. Through its proprietary technology, its voice AI delivers speed and accuracy in numerous languages to product creators and service providers across retail, financial services, healthcare, automotive, smart devices, and restaurants via AI-driven products, such as Smart Answering, Smart Ordering, Dynamic Drive Thru, and Amelia AI Agents. Along with SoundHound Chat AI, a voice assistant with integrated Generative AI, it powers various products and services, and processes billions of interactions each year for businesses. Its developer platform, Houndify, is an open-access platform that allows developers to leverage its Voice AI technology and a library of over 100 content domains, including commonly used domains for points of interest, weather, flight status, sports and more.</v>
     <v>842</v>
@@ -1730,24 +1736,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>5400 Betsy Ross Drive, SANTA CLARA, CA, 95054 US</v>
-    <v>9.3800000000000008</v>
+    <v>10.4</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999886851561</v>
+    <v>45833.999971284378</v>
     <v>35</v>
-    <v>9.01</v>
-    <v>3655782000</v>
+    <v>9.52</v>
+    <v>3844597251</v>
     <v>SOUNDHOUND AI, INC.</v>
     <v>SOUNDHOUND AI, INC.</v>
-    <v>9.08</v>
+    <v>10.119999999999999</v>
     <v>0</v>
-    <v>9.4700000000000006</v>
-    <v>9.1</v>
+    <v>9.82</v>
+    <v>9.57</v>
     <v>401734300</v>
     <v>SOUN</v>
     <v>SOUNDHOUND AI, INC. (XNAS:SOUN)</v>
-    <v>62954</v>
-    <v>36647911</v>
+    <v>121445</v>
+    <v>31665449</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -1768,12 +1774,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>1262.81</v>
+    <v>5</v>
+    <v>1297.9999</v>
     <v>587.04</v>
-    <v>1.5887</v>
-    <v>-2.88</v>
-    <v>-2.3699999999999997E-3</v>
+    <v>1.5892999999999999</v>
+    <v>-3.86</v>
+    <v>-3.0180000000000003E-3</v>
     <v>USD</v>
     <v>Netflix, Inc. is a provider of entertainment services. The Company acquires, licenses and produces content, including original programming. It provides paid memberships in over 190 countries offering television (TV) series, films and games across a variety of genres and languages. It allows members to play, pause and resume watching as much as they want, anytime, anywhere, and can change their plans at any time. The Company offers members the ability to receive streaming content through a host of Internet-connected devices, including TVs, digital video players, TV set-top boxes and mobile devices. It is engaged in scaling its streaming service, such as introducing games and advertising on its service, as well as offering live programming. It is developing technology and utilizing third-party cloud computing, technology and other services. The Company is also engaged in scaling its own studio operations to produce original content.</v>
     <v>14000</v>
@@ -1781,24 +1787,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>121 Albright Way, LOS GATOS, CA, 95032 US</v>
-    <v>1220.6199999999999</v>
+    <v>1297.9999</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999954617968</v>
+    <v>45833.999853344532</v>
     <v>38</v>
-    <v>1201.8900000000001</v>
-    <v>515856200000</v>
+    <v>1273.81</v>
+    <v>542709800325</v>
     <v>NETFLIX, INC.</v>
     <v>NETFLIX, INC.</v>
-    <v>1206.5899999999999</v>
-    <v>57.275100000000002</v>
-    <v>1215.03</v>
-    <v>1212.1500000000001</v>
+    <v>1286.8399999999999</v>
+    <v>60.256700000000002</v>
+    <v>1279.1099999999999</v>
+    <v>1275.25</v>
     <v>425571300</v>
     <v>NFLX</v>
     <v>NETFLIX, INC. (XNAS:NFLX)</v>
-    <v>1613</v>
-    <v>3135515</v>
+    <v>2317</v>
+    <v>2707317</v>
     <v>1997</v>
   </rv>
   <rv s="2">
@@ -1815,12 +1821,12 @@
     <v>13</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>188.75</v>
     <v>80</v>
     <v>2.113</v>
-    <v>-3.07</v>
-    <v>-2.2147E-2</v>
+    <v>0.9</v>
+    <v>5.7540000000000004E-3</v>
     <v>USD</v>
     <v>Arm Holdings plc is engaged in operating a global computing platform. It architects, develops, and licenses IP solutions for CPUs, GPUs, NPUs and interconnect technologies, which is relied on by semiconductor companies and OEMs to develop their products. Its principal operations are the licensing, marketing, research and development of microprocessors, systems intellectual property (IP), graphics processing units, physical IP and associated systems IP, software, tools and other related services. Its primary product offerings are CPU products that address diverse performance, power, and cost requirements. Its complementary products, such as graphics processing units (GPUs) that accelerate the display of complex graphics onto a screen and can also be used for other mathematical applications, System IP, and compute platforms are also available as well as development tools and a software ecosystem to enable high-performance system-level creation for a range of devices and applications.</v>
     <v>8330</v>
@@ -1828,23 +1834,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>110 Fulbourn Road, CAMBRIDGE, CAMBRIDGESHIRE, CB1 9NJ GB</v>
-    <v>138.52000000000001</v>
+    <v>159.88</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.999829524997</v>
-    <v>134.57</v>
-    <v>143583200000</v>
+    <v>45833.99923092578</v>
+    <v>156.68</v>
+    <v>166632819840</v>
     <v>ARM HOLDINGS PLC</v>
     <v>ARM HOLDINGS PLC</v>
-    <v>135.81</v>
-    <v>181.93170000000001</v>
-    <v>138.62</v>
-    <v>135.55000000000001</v>
+    <v>157.11000000000001</v>
+    <v>211.13740000000001</v>
+    <v>156.41</v>
+    <v>157.31</v>
     <v>1059264000</v>
     <v>ARM</v>
     <v>ARM HOLDINGS PLC (XNAS:ARM)</v>
-    <v>3601</v>
-    <v>5265994</v>
+    <v>21903</v>
+    <v>4299040</v>
     <v>2018</v>
   </rv>
   <rv s="2">
@@ -1865,12 +1871,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>207.05</v>
     <v>140.53</v>
-    <v>1.0138</v>
-    <v>-1.03</v>
-    <v>-5.8620000000000009E-3</v>
+    <v>1.0044999999999999</v>
+    <v>3.91</v>
+    <v>2.3445000000000001E-2</v>
     <v>USD</v>
     <v>Alphabet Inc. is a holding company. The Company's segments include Google Services, Google Cloud, and Other Bets. The Google Services segment includes products and services such as ads, Android, Chrome, devices, Google Maps, Google Play, Search, and YouTube. The Google Cloud segment includes infrastructure and platform services, collaboration tools, and other services for enterprise customers. Its Other Bets segment is engaged in the sale of healthcare-related services and Internet services. Its Google Cloud provides enterprise-ready cloud services, including Google Cloud Platform and Google Workspace. Google Cloud Platform provides access to solutions such as artificial intelligence (AI) offerings, including its AI infrastructure, Vertex AI platform, and Gemini for Google Cloud; cybersecurity, and data and analytics. Google Workspace includes cloud-based communication and collaboration tools for enterprises, such as Calendar, Gmail, Docs, Drive, and Meet.</v>
     <v>185719</v>
@@ -1878,24 +1884,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1600 Amphitheatre Parkway, MOUNTAIN VIEW, CA, 94043 US</v>
-    <v>177.13</v>
+    <v>172.36</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999880253905</v>
+    <v>45833.999933032028</v>
     <v>43</v>
-    <v>172.38499999999999</v>
-    <v>2126226000000</v>
+    <v>167.55</v>
+    <v>2029049000000</v>
     <v>ALPHABET INC.</v>
     <v>ALPHABET INC.</v>
-    <v>172.44</v>
-    <v>19.470800000000001</v>
-    <v>175.7</v>
-    <v>174.67</v>
+    <v>167.63</v>
+    <v>19.026</v>
+    <v>166.77</v>
+    <v>170.68</v>
     <v>12135000000</v>
     <v>GOOGL</v>
     <v>ALPHABET INC. (XNAS:GOOGL)</v>
-    <v>25132</v>
-    <v>41703536</v>
+    <v>191380</v>
+    <v>40958884</v>
     <v>2015</v>
   </rv>
   <rv s="2">
@@ -1917,11 +1923,11 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>717.87</v>
+    <v>759.17</v>
     <v>288.07</v>
-    <v>1.6623000000000001</v>
-    <v>8.0299999999999994</v>
-    <v>1.1425000000000001E-2</v>
+    <v>1.6728000000000001</v>
+    <v>-13.61</v>
+    <v>-1.8148999999999998E-2</v>
     <v>USD</v>
     <v>Spotify Technology SA a Luxembourg-based company, which offers digital music-streaming services. The Company enables users to discover new releases, which includes the latest singles and albums; playlists, which includes ready-made playlists put together by music fans and experts, and over millions of songs so that users can play their favorites, discover new tracks and build a personalized collection. Its users can either select Spotify Free, which includes only shuffle play or Spotify Premium, which encompasses a range of features, such as shuffle play, advertisement free, unlimited skips, listen offline, play any track and audio. The Company operates through a number of subsidiaries, including Spotify LTD and is present in over 20 countries. Its service offers a music listening experience without commercial breaks.</v>
     <v>7691</v>
@@ -1929,24 +1935,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>42-44, avenue de la Gare, LUXEMBOURG, 1610 LU</v>
-    <v>710.89</v>
+    <v>759.17</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999479837497</v>
+    <v>45833.999248135937</v>
     <v>46</v>
-    <v>691.21</v>
-    <v>145516000000</v>
+    <v>735.60649999999998</v>
+    <v>150725837730</v>
     <v>Spotify Technology SA</v>
     <v>Spotify Technology SA</v>
-    <v>694.76</v>
-    <v>117.45910000000001</v>
-    <v>702.82</v>
-    <v>710.85</v>
+    <v>752.7</v>
+    <v>121.6644</v>
+    <v>749.91</v>
+    <v>736.3</v>
     <v>204707100</v>
     <v>SPOT</v>
     <v>Spotify Technology SA (XNYS:SPOT)</v>
-    <v>254</v>
-    <v>1877660</v>
+    <v>612</v>
+    <v>1684090</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -1967,37 +1973,37 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>157.535</v>
+    <v>5</v>
+    <v>144.07</v>
     <v>61.54</v>
-    <v>1.2795000000000001</v>
-    <v>-0.57999999999999996</v>
-    <v>-4.9919999999999999E-3</v>
+    <v>1.3252999999999999</v>
+    <v>-0.66</v>
+    <v>-5.1600000000000005E-3</v>
     <v>USD</v>
     <v>Micron Technology, Inc. provides memory and storage solutions. The Company delivers a portfolio of high-performance dynamic random-access memory (DRAM), NAND, and NOR memory and storage products through its Micron and Crucial brands. The Company's products enable advancing in artificial intelligence (AI) and compute-intensive applications. Its segments include Compute and Networking Business Unit (CNBU), Mobile Business Unit (MBU), Embedded Business Unit (EBU), and Storage Business Unit (SBU). CNBU segment includes memory products and solutions sold into the data center, PC, graphics, and networking markets. MBU segment includes memory and storage products sold into the smartphone and other mobile-device markets. EBU segment includes memory and storage products and solutions sold into the intelligent edge through the automotive, industrial, and consumer embedded markets. SBU segment includes SSDs and component-level storage solutions sold into the data center, PC, and consumer markets.</v>
     <v>48000</v>
     <v>Nasdaq Stock Market</v>
     <v>XNAS</v>
     <v>XNAS</v>
-    <v>PO BOX 6, 8000 S FEDERAL WAY, BOISE, ID, 83716-9632 US</v>
-    <v>117.1</v>
+    <v>8000 S Federal Way, Po Box 6, BOISE, ID, 83716-9632 US</v>
+    <v>127.5</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.999961191403</v>
+    <v>45833.999999224216</v>
     <v>49</v>
-    <v>113.66</v>
-    <v>129191300000</v>
+    <v>125.62</v>
+    <v>142211037000</v>
     <v>MICRON TECHNOLOGY, INC.</v>
     <v>MICRON TECHNOLOGY, INC.</v>
-    <v>113.8</v>
-    <v>27.945699999999999</v>
-    <v>116.18</v>
-    <v>115.6</v>
+    <v>126.61</v>
+    <v>23.0671</v>
+    <v>127.91</v>
+    <v>127.25</v>
     <v>1117572000</v>
     <v>MU</v>
     <v>MICRON TECHNOLOGY, INC. (XNAS:MU)</v>
-    <v>13870</v>
-    <v>19423056</v>
+    <v>385832</v>
+    <v>19332364</v>
     <v>1984</v>
   </rv>
   <rv s="2">
@@ -2018,12 +2024,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>1110.0899999999999</v>
     <v>578.51</v>
-    <v>1.7322</v>
-    <v>-25.21</v>
-    <v>-3.2065000000000003E-2</v>
+    <v>1.74</v>
+    <v>1.88</v>
+    <v>2.3110000000000001E-3</v>
     <v>USD</v>
     <v>ASML Holding N.V. is a holding company based in the Netherlands. The Company operates through its subsidiaries in the Netherlands, the United States, Italy, France, Germany, the United Kingdom, Ireland, Belgium, South Korea, Taiwan, Singapore, China, Hong Kong, Japan, Malaysia and Israel. The Company operates through one business segment which is engage in development, production, marketing, sales, upgrading and servicing of advanced semiconductor equipment systems, consisting of lithography, metrology and inspection systems. The Company offers TWINSCAN systems, equipped with lithography system with a mercury lamp as light source (i-line), Krypton Fluoride (KrF) and Argon Fluoride (ArF) light sources for processing wafers for manufacturing environments for which imaging at a small resolution is required. TWINSCAN systems also include immersion lithography systems (TWINSCAN immersion systems).</v>
     <v>43129</v>
@@ -2031,24 +2037,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>De Run 6501, VELDHOVEN, NOORD-BRABANT, 5504 DR NL</v>
-    <v>772.93</v>
+    <v>819.54</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45821.999885138284</v>
+    <v>45833.999871631248</v>
     <v>52</v>
-    <v>759.87</v>
-    <v>303174800000</v>
+    <v>806.22</v>
+    <v>315206800000</v>
     <v>ASML Holding NV</v>
     <v>ASML Holding NV</v>
-    <v>766.89</v>
-    <v>31.763100000000001</v>
-    <v>786.21</v>
-    <v>761</v>
+    <v>816.745</v>
+    <v>34.027000000000001</v>
+    <v>813.36</v>
+    <v>815.24</v>
     <v>393830700</v>
     <v>ASML</v>
     <v>ASML Holding NV (XNAS:ASML)</v>
-    <v>1099</v>
-    <v>1304779</v>
+    <v>17604</v>
+    <v>1367373</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -2089,38 +2095,38 @@
     <v>16</v>
     <v>17</v>
     <v>Finance</v>
-    <v>4</v>
-    <v>216.59989999999999</v>
+    <v>5</v>
+    <v>216.9299</v>
     <v>118.86</v>
-    <v>1.3214999999999999</v>
-    <v>15.36</v>
-    <v>7.6853999999999992E-2</v>
+    <v>1.3593</v>
+    <v>-4.55</v>
+    <v>-2.1135999999999999E-2</v>
     <v>USD</v>
     <v>Oracle Corporation offers integrated suites of applications plus secure, autonomous infrastructure in the Oracle Cloud. The Company's segments include cloud and license, hardware, and services. The cloud and license segment markets, sells and delivers a broad spectrum of enterprise applications and infrastructure technologies through its cloud and license offerings. The hardware segment provides a broad selection of enterprise hardware products and hardware-related software products including Oracle Engineered Systems, servers, storage, operating systems, virtualization, management and other hardware-related software and related hardware support. The services segment helps customers and partners maximize the performance of their investments in Oracle applications and infrastructure technologies. Its products and services are delivered worldwide through a variety of flexible and interoperable IT deployment models. These models include on-premise, cloud-based and hybrid deployments.</v>
-    <v>159000</v>
+    <v>162000</v>
     <v>New York Stock Exchange</v>
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2300 Oracle Way, AUSTIN, TX, 78741 US</v>
-    <v>216.59989999999999</v>
+    <v>216.9299</v>
     <v>58</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45821.999981990622</v>
+    <v>45833.999729941403</v>
     <v>59</v>
-    <v>201.2</v>
-    <v>603527300000</v>
+    <v>210.23</v>
+    <v>591877289760</v>
     <v>ORACLE CORPORATION</v>
     <v>ORACLE CORPORATION</v>
-    <v>201.58</v>
-    <v>49.579799999999999</v>
-    <v>199.86</v>
-    <v>215.22</v>
-    <v>2804234000</v>
+    <v>214.93989999999999</v>
+    <v>48.533900000000003</v>
+    <v>215.27</v>
+    <v>210.72</v>
+    <v>2808833000</v>
     <v>ORCL</v>
     <v>ORACLE CORPORATION (XNYS:ORCL)</v>
-    <v>21263</v>
-    <v>10520531</v>
+    <v>8807</v>
+    <v>14750126</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -2141,12 +2147,12 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>972.53</v>
     <v>677.09119999999996</v>
-    <v>0.39410000000000001</v>
-    <v>7.33</v>
-    <v>9.0270000000000003E-3</v>
+    <v>0.3972</v>
+    <v>14.22</v>
+    <v>1.8276000000000001E-2</v>
     <v>USD</v>
     <v>Eli Lilly and Company is a medicine company, which discovers, develops, manufactures and markets products in the human pharmaceutical products segment. Its cardiometabolic health products include Basaglar; Humalog, Humalog Mix 75/25, Humalog U-100, Humalog U-200, Humalog Mix 50/50, insulin lispro, and others; Humulin, Humulin 70/30, and others; Jardiance; Mounjaro; Trulicity, and Zepbound. Its oncology products include Cyramza, Erbitux, Tyvyt, and Verzenio. Its immunology products include Ebglyss, Olumiant, Omvoh, and Taltz. Its neuroscience products include Emgality and Kisunla. The Company, through its subsidiary, POINT Biopharma Global Inc., is engaged in radiopharmaceutical discovery, development, and manufacturing efforts, as well as clinical and pre-clinical radioligand therapies in development for the treatment of cancer. It is also developing an oral small molecule inhibitor of a4b7 integrin for inflammatory bowel disease (IBD). It also owns a lead therapeutic molecule, FXR314.</v>
     <v>47000</v>
@@ -2154,24 +2160,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Lilly Corporate Ctr, Drop Code 1094, INDIANAPOLIS, IN, 46285 US</v>
-    <v>825</v>
+    <v>798.95</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45821.999837418749</v>
+    <v>45833.999944814066</v>
     <v>62</v>
-    <v>808.1001</v>
-    <v>776536700000</v>
+    <v>773.59500000000003</v>
+    <v>750890995110</v>
     <v>ELI LILLY AND COMPANY</v>
     <v>ELI LILLY AND COMPANY</v>
-    <v>810.33500000000004</v>
-    <v>66.611099999999993</v>
-    <v>812.03</v>
-    <v>819.36</v>
+    <v>779</v>
+    <v>64.411199999999994</v>
+    <v>778.08</v>
+    <v>792.3</v>
     <v>947735700</v>
     <v>LLY</v>
     <v>ELI LILLY AND COMPANY (XNYS:LLY)</v>
-    <v>1187</v>
-    <v>4124731</v>
+    <v>1427</v>
+    <v>3424512</v>
     <v>1901</v>
   </rv>
   <rv s="2">
@@ -2656,17 +2662,17 @@
       <v>4</v>
     </spb>
     <spb s="4">
+      <v>Delayed 15 minutes</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="4">
       <v>Real-Time Nasdaq Last Sale</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
-      <v>GMT</v>
-    </spb>
-    <spb s="4">
-      <v>Delayed 15 minutes</v>
-      <v>from previous close</v>
-      <v>from previous close</v>
-      <v>Source: Nasdaq</v>
       <v>GMT</v>
     </spb>
     <spb s="0">
@@ -2978,8 +2984,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8E4D55F-7633-495E-A517-D2E57B09B7A7}" name="OrdersYigaelIsrael" displayName="OrdersYigaelIsrael" ref="A1:N173" totalsRowShown="0">
-  <autoFilter ref="A1:N173" xr:uid="{D8E4D55F-7633-495E-A517-D2E57B09B7A7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8E4D55F-7633-495E-A517-D2E57B09B7A7}" name="OrdersYigaelIsrael" displayName="OrdersYigaelIsrael" ref="A1:N178" totalsRowShown="0">
+  <autoFilter ref="A1:N178" xr:uid="{D8E4D55F-7633-495E-A517-D2E57B09B7A7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N171">
     <sortCondition ref="C1:C171"/>
   </sortState>
@@ -3390,12 +3396,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB241026-986E-4717-8246-2FB0114F2590}">
-  <dimension ref="A1:W173"/>
+  <dimension ref="A1:W178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="N173" sqref="N173"/>
+      <selection pane="bottomLeft" activeCell="N178" sqref="N178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,14 +3475,14 @@
       </c>
       <c r="Q1" s="18">
         <f>SUM(OrdersYigaelIsrael[P&amp;L])</f>
-        <v>163257.05325924436</v>
+        <v>163737.27091042936</v>
       </c>
       <c r="S1" t="s">
         <v>14</v>
       </c>
       <c r="T1">
         <f>(Q1/W1)*100</f>
-        <v>15.697793582619651</v>
+        <v>15.743968356772054</v>
       </c>
       <c r="V1" t="s">
         <v>15</v>
@@ -11630,7 +11636,7 @@
       </c>
       <c r="Q169" s="20">
         <f>SUMIFS(OrdersYigaelIsrael[P&amp;L], OrdersYigaelIsrael[Year-Month], "2025-06")</f>
-        <v>14154.535288154955</v>
+        <v>14634.752939339965</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.25">
@@ -11658,10 +11664,6 @@
       <c r="L170">
         <v>2570.58</v>
       </c>
-      <c r="N170">
-        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
-        <v>157360.39906724438</v>
-      </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
@@ -11670,13 +11672,19 @@
       <c r="B171" s="1">
         <v>45806</v>
       </c>
+      <c r="C171" s="1">
+        <v>45826</v>
+      </c>
       <c r="D171" t="str">
         <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
-        <v>1900-01</v>
+        <v>2025-06</v>
       </c>
       <c r="E171" s="2">
         <v>29770</v>
       </c>
+      <c r="F171" s="2">
+        <v>30030</v>
+      </c>
       <c r="G171" s="21">
         <v>839</v>
       </c>
@@ -11684,11 +11692,26 @@
         <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
         <v>249770.3</v>
       </c>
+      <c r="I171">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>251951.7</v>
+      </c>
       <c r="J171">
         <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
-        <v>174.83920999999998</v>
-      </c>
-      <c r="K171" s="19"/>
+        <v>351.2054</v>
+      </c>
+      <c r="K171" s="19">
+        <f>(OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]-OrdersYigaelIsrael[[#This Row],[Commission]]+OrdersYigaelIsrael[[#This Row],[Dividand]])/OrdersYigaelIsrael[[#This Row],[Buy Value]]</f>
+        <v>7.3275109170306612E-3</v>
+      </c>
+      <c r="M171">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Dividand]]-OrdersYigaelIsrael[[#This Row],[Commission]]</f>
+        <v>1830.1946000000232</v>
+      </c>
+      <c r="N171">
+        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
+        <v>159190.59366724439</v>
+      </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
@@ -11735,7 +11758,7 @@
       </c>
       <c r="N172">
         <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
-        <v>163257.05325924436</v>
+        <v>165087.24785924438</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
@@ -11745,13 +11768,19 @@
       <c r="B173" s="1">
         <v>45824</v>
       </c>
-      <c r="D173" s="22" t="str">
-        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
-        <v>1900-01</v>
+      <c r="C173" s="1">
+        <v>45825</v>
+      </c>
+      <c r="D173" t="str">
+        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
+        <v>2025-06</v>
       </c>
       <c r="E173" s="2">
         <v>20729.403999999999</v>
       </c>
+      <c r="F173" s="2">
+        <v>21140</v>
+      </c>
       <c r="G173" s="21">
         <v>1594</v>
       </c>
@@ -11759,12 +11788,246 @@
         <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
         <v>330426.69975999999</v>
       </c>
-      <c r="J173" s="22">
-        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
-        <v>231.29868983199998</v>
-      </c>
-      <c r="K173" s="19"/>
-      <c r="N173" s="22"/>
+      <c r="I173">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>336971.6</v>
+      </c>
+      <c r="J173">
+        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
+        <v>467.17880983199996</v>
+      </c>
+      <c r="K173" s="19">
+        <f>(OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]-OrdersYigaelIsrael[[#This Row],[Commission]]+OrdersYigaelIsrael[[#This Row],[Dividand]])/OrdersYigaelIsrael[[#This Row],[Buy Value]]</f>
+        <v>1.8393554257517451E-2</v>
+      </c>
+      <c r="M173">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Dividand]]-OrdersYigaelIsrael[[#This Row],[Commission]]</f>
+        <v>6077.7214301679878</v>
+      </c>
+      <c r="N173">
+        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
+        <v>171164.96928941237</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>17</v>
+      </c>
+      <c r="B174" s="1">
+        <v>45827</v>
+      </c>
+      <c r="C174" s="1">
+        <v>45830</v>
+      </c>
+      <c r="D174" t="str">
+        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
+        <v>2025-06</v>
+      </c>
+      <c r="E174" s="2">
+        <v>5940</v>
+      </c>
+      <c r="F174" s="2">
+        <v>6060</v>
+      </c>
+      <c r="G174" s="21">
+        <v>5054</v>
+      </c>
+      <c r="H174">
+        <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>300207.59999999998</v>
+      </c>
+      <c r="I174">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>306272.40000000002</v>
+      </c>
+      <c r="J174">
+        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
+        <v>424.536</v>
+      </c>
+      <c r="K174" s="19">
+        <f>(OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]-OrdersYigaelIsrael[[#This Row],[Commission]]+OrdersYigaelIsrael[[#This Row],[Dividand]])/OrdersYigaelIsrael[[#This Row],[Buy Value]]</f>
+        <v>1.8787878787878944E-2</v>
+      </c>
+      <c r="M174">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Dividand]]-OrdersYigaelIsrael[[#This Row],[Commission]]</f>
+        <v>5640.2640000000465</v>
+      </c>
+      <c r="N174">
+        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
+        <v>176805.23328941243</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>106</v>
+      </c>
+      <c r="B175" s="1">
+        <v>45827</v>
+      </c>
+      <c r="C175" s="1">
+        <v>45830</v>
+      </c>
+      <c r="D175" t="str">
+        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
+        <v>2025-06</v>
+      </c>
+      <c r="E175" s="2">
+        <v>12060</v>
+      </c>
+      <c r="F175" s="2">
+        <v>12408</v>
+      </c>
+      <c r="G175" s="21">
+        <v>2487</v>
+      </c>
+      <c r="H175">
+        <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>299932.2</v>
+      </c>
+      <c r="I175">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>308586.96000000002</v>
+      </c>
+      <c r="J175">
+        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
+        <v>425.96341200000001</v>
+      </c>
+      <c r="K175" s="19">
+        <f>(OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]-OrdersYigaelIsrael[[#This Row],[Commission]]+OrdersYigaelIsrael[[#This Row],[Dividand]])/OrdersYigaelIsrael[[#This Row],[Buy Value]]</f>
+        <v>2.7435522388059734E-2</v>
+      </c>
+      <c r="M175">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Dividand]]-OrdersYigaelIsrael[[#This Row],[Commission]]</f>
+        <v>8228.7965880000102</v>
+      </c>
+      <c r="N175">
+        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
+        <v>185034.02987741242</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>42</v>
+      </c>
+      <c r="B176" s="1">
+        <v>45830</v>
+      </c>
+      <c r="C176" s="1"/>
+      <c r="D176" t="str">
+        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
+        <v>1900-01</v>
+      </c>
+      <c r="E176" s="2">
+        <v>52840</v>
+      </c>
+      <c r="G176" s="21">
+        <v>48</v>
+      </c>
+      <c r="H176">
+        <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>25363.200000000001</v>
+      </c>
+      <c r="J176">
+        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
+        <v>17.754239999999999</v>
+      </c>
+      <c r="K176" s="19"/>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>25</v>
+      </c>
+      <c r="B177" s="1">
+        <v>45831</v>
+      </c>
+      <c r="C177" s="1">
+        <v>45834</v>
+      </c>
+      <c r="D177" t="str">
+        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
+        <v>2025-06</v>
+      </c>
+      <c r="E177" s="2">
+        <v>6420</v>
+      </c>
+      <c r="F177" s="2">
+        <v>6180.4369999999999</v>
+      </c>
+      <c r="G177" s="21">
+        <v>4687</v>
+      </c>
+      <c r="H177">
+        <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>300905.40000000002</v>
+      </c>
+      <c r="I177">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>289677.08218999999</v>
+      </c>
+      <c r="J177">
+        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
+        <v>413.40773753299999</v>
+      </c>
+      <c r="K177" s="19">
+        <f>(OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]-OrdersYigaelIsrael[[#This Row],[Commission]]+OrdersYigaelIsrael[[#This Row],[Dividand]])/OrdersYigaelIsrael[[#This Row],[Buy Value]]</f>
+        <v>-3.8688988457944044E-2</v>
+      </c>
+      <c r="M177">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Dividand]]-OrdersYigaelIsrael[[#This Row],[Commission]]</f>
+        <v>-11641.725547533037</v>
+      </c>
+      <c r="N177">
+        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
+        <v>173392.30432987938</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>35</v>
+      </c>
+      <c r="B178" s="1">
+        <v>45831</v>
+      </c>
+      <c r="C178" s="1">
+        <v>45834</v>
+      </c>
+      <c r="D178" s="22" t="str">
+        <f>TEXT(OrdersYigaelIsrael[[#This Row],[Sell Date]],"yyyy-mm")</f>
+        <v>2025-06</v>
+      </c>
+      <c r="E178" s="2">
+        <v>5968.9759999999997</v>
+      </c>
+      <c r="F178" s="2">
+        <v>5784.9489999999996</v>
+      </c>
+      <c r="G178" s="23">
+        <v>5022</v>
+      </c>
+      <c r="H178">
+        <f>OrdersYigaelIsrael[[#This Row],[Buy Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>299761.97472</v>
+      </c>
+      <c r="I178">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Price]]*OrdersYigaelIsrael[[#This Row],[Amount]]/100</f>
+        <v>290520.13877999998</v>
+      </c>
+      <c r="J178" s="22">
+        <f>(OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Sell Value]])*0.0007</f>
+        <v>413.19747945</v>
+      </c>
+      <c r="K178" s="19">
+        <f>(OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]-OrdersYigaelIsrael[[#This Row],[Commission]]+OrdersYigaelIsrael[[#This Row],[Dividand]])/OrdersYigaelIsrael[[#This Row],[Buy Value]]</f>
+        <v>-3.2208999918914127E-2</v>
+      </c>
+      <c r="M178">
+        <f>OrdersYigaelIsrael[[#This Row],[Sell Value]]-OrdersYigaelIsrael[[#This Row],[Buy Value]]+OrdersYigaelIsrael[[#This Row],[Dividand]]-OrdersYigaelIsrael[[#This Row],[Commission]]</f>
+        <v>-9655.0334194500192</v>
+      </c>
+      <c r="N178" s="22">
+        <f>SUM(INDEX(OrdersYigaelIsrael[P&amp;L],1):OrdersYigaelIsrael[[#This Row],[P&amp;L]])</f>
+        <v>163737.27091042936</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11883,7 +12146,7 @@
       </c>
       <c r="G2" s="10" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>53.52</v>
+        <v>51.92</v>
       </c>
       <c r="H2" s="6">
         <v>280</v>
@@ -11898,7 +12161,7 @@
       </c>
       <c r="K2" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>14985.6</v>
+        <v>14537.6</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="7"/>
@@ -11937,7 +12200,7 @@
       </c>
       <c r="G3" s="10" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H3" s="6">
         <v>70</v>
@@ -11952,7 +12215,7 @@
       </c>
       <c r="K3" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>9937.9</v>
+        <v>10801.7</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="7"/>
@@ -11985,7 +12248,7 @@
       </c>
       <c r="G4" s="10" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>52.26</v>
+        <v>51.48</v>
       </c>
       <c r="H4" s="6">
         <v>1180</v>
@@ -12000,7 +12263,7 @@
       </c>
       <c r="K4" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>61666.799999999996</v>
+        <v>60746.399999999994</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="7"/>
@@ -12033,7 +12296,7 @@
       </c>
       <c r="G5" s="10" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>38.090000000000003</v>
+        <v>42.84</v>
       </c>
       <c r="H5" s="6">
         <v>750</v>
@@ -12048,7 +12311,7 @@
       </c>
       <c r="K5" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>28567.500000000004</v>
+        <v>32130.000000000004</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="7"/>
@@ -12087,7 +12350,7 @@
       </c>
       <c r="G6" s="10" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>97.17</v>
+        <v>102.84</v>
       </c>
       <c r="H6" s="6">
         <v>400</v>
@@ -12102,7 +12365,7 @@
       </c>
       <c r="K6" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>38868</v>
+        <v>41136</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="7"/>
@@ -12143,7 +12406,7 @@
       </c>
       <c r="G7" s="10" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H7" s="6">
         <v>70</v>
@@ -12158,7 +12421,7 @@
       </c>
       <c r="K7" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>9937.9</v>
+        <v>10801.7</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="7"/>
@@ -12195,7 +12458,7 @@
       </c>
       <c r="G8" s="10" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H8" s="6">
         <v>103</v>
@@ -12210,7 +12473,7 @@
       </c>
       <c r="K8" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>14622.91</v>
+        <v>15893.93</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="7"/>
@@ -12249,7 +12512,7 @@
       </c>
       <c r="G9" s="8" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>137.4</v>
+        <v>142.9</v>
       </c>
       <c r="H9" s="6">
         <v>1700</v>
@@ -12264,7 +12527,7 @@
       </c>
       <c r="K9" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>233580</v>
+        <v>242930</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="7"/>
@@ -12276,7 +12539,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
         <f ca="1">Realized_and_Unrealized_Profit_Yigael_USA*USD_ILS_Price</f>
-        <v>96609.116981393978</v>
+        <v>92536.174033163974</v>
       </c>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
@@ -12304,7 +12567,7 @@
       </c>
       <c r="G10" s="8" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>325.31</v>
+        <v>327.55</v>
       </c>
       <c r="H10" s="6">
         <v>200</v>
@@ -12319,7 +12582,7 @@
       </c>
       <c r="K10" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>65062</v>
+        <v>65510</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="7"/>
@@ -12356,7 +12619,7 @@
       </c>
       <c r="G11" s="8" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H11" s="6">
         <v>110</v>
@@ -12371,7 +12634,7 @@
       </c>
       <c r="K11" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>15616.7</v>
+        <v>16974.099999999999</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="7"/>
@@ -12410,7 +12673,7 @@
       </c>
       <c r="G12" s="8" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>20.14</v>
+        <v>22.2</v>
       </c>
       <c r="H12" s="6">
         <v>1300</v>
@@ -12425,7 +12688,7 @@
       </c>
       <c r="K12" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>26182</v>
+        <v>28860</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="7"/>
@@ -12464,7 +12727,7 @@
       </c>
       <c r="G13" s="8" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>116.16</v>
+        <v>143.4</v>
       </c>
       <c r="H13" s="6">
         <v>200</v>
@@ -12479,7 +12742,7 @@
       </c>
       <c r="K13" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>23232</v>
+        <v>28680</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="7"/>
@@ -12518,7 +12781,7 @@
       </c>
       <c r="G14" s="8" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>211.1</v>
+        <v>222.74</v>
       </c>
       <c r="H14" s="6">
         <v>423</v>
@@ -12533,7 +12796,7 @@
       </c>
       <c r="K14" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>89295.3</v>
+        <v>94219.02</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="7"/>
@@ -12573,7 +12836,7 @@
       </c>
       <c r="G15" s="8" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H15" s="6">
         <v>30</v>
@@ -12588,7 +12851,7 @@
       </c>
       <c r="K15" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>1246.8000000000002</v>
+        <v>1398.3</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="7"/>
@@ -12625,7 +12888,7 @@
       </c>
       <c r="G16" s="8" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H16" s="6">
         <v>20</v>
@@ -12640,7 +12903,7 @@
       </c>
       <c r="K16" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>831.2</v>
+        <v>932.2</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="7"/>
@@ -12677,7 +12940,7 @@
       </c>
       <c r="G17" s="8" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H17" s="6">
         <v>40</v>
@@ -12692,7 +12955,7 @@
       </c>
       <c r="K17" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>1662.4</v>
+        <v>1864.4</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="7"/>
@@ -12707,7 +12970,7 @@
       </c>
       <c r="R17" s="6" cm="1">
         <f t="array" aca="1" ref="R17" ca="1">_FV(USD_NIS,"Price",TRUE)</f>
-        <v>3.5461</v>
+        <v>3.3965999999999998</v>
       </c>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -12734,7 +12997,7 @@
       </c>
       <c r="G18" s="8" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>9.1</v>
+        <v>9.57</v>
       </c>
       <c r="H18" s="6">
         <v>6100</v>
@@ -12749,7 +13012,7 @@
       </c>
       <c r="K18" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>55510</v>
+        <v>58377</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="7"/>
@@ -12786,7 +13049,7 @@
       </c>
       <c r="G19" s="8" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>9.1</v>
+        <v>9.57</v>
       </c>
       <c r="H19" s="6">
         <v>5400</v>
@@ -12801,7 +13064,7 @@
       </c>
       <c r="K19" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>49140</v>
+        <v>51678</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="7"/>
@@ -12838,7 +13101,7 @@
       </c>
       <c r="G20" s="8" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>137.4</v>
+        <v>142.9</v>
       </c>
       <c r="H20" s="6">
         <v>1200</v>
@@ -12853,7 +13116,7 @@
       </c>
       <c r="K20" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>164880</v>
+        <v>171480</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="7"/>
@@ -12889,7 +13152,7 @@
       </c>
       <c r="G21" s="8" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>137.4</v>
+        <v>142.9</v>
       </c>
       <c r="H21" s="6">
         <v>1200</v>
@@ -12904,7 +13167,7 @@
       </c>
       <c r="K21" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>164880</v>
+        <v>171480</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="7"/>
@@ -12941,7 +13204,7 @@
       </c>
       <c r="G22" s="8" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>137.4</v>
+        <v>142.9</v>
       </c>
       <c r="H22" s="6">
         <v>1300</v>
@@ -12956,7 +13219,7 @@
       </c>
       <c r="K22" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>178620</v>
+        <v>185770</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="7"/>
@@ -12993,7 +13256,7 @@
       </c>
       <c r="G23" s="8" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>116.16</v>
+        <v>143.4</v>
       </c>
       <c r="H23" s="6">
         <v>150</v>
@@ -13008,7 +13271,7 @@
       </c>
       <c r="K23" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>17424</v>
+        <v>21510</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="7"/>
@@ -13045,7 +13308,7 @@
       </c>
       <c r="G24" s="8" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>1212.1500000000001</v>
+        <v>1275.25</v>
       </c>
       <c r="H24" s="6">
         <v>50</v>
@@ -13060,7 +13323,7 @@
       </c>
       <c r="K24" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>60607.500000000007</v>
+        <v>63762.5</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="7"/>
@@ -13097,7 +13360,7 @@
       </c>
       <c r="G25" s="8" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H25" s="6">
         <v>40</v>
@@ -13112,7 +13375,7 @@
       </c>
       <c r="K25" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>5678.8</v>
+        <v>6172.4</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="7"/>
@@ -13149,7 +13412,7 @@
       </c>
       <c r="G26" s="8" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>9.1</v>
+        <v>9.57</v>
       </c>
       <c r="H26" s="6">
         <v>10700</v>
@@ -13164,7 +13427,7 @@
       </c>
       <c r="K26" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>97370</v>
+        <v>102399</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="7"/>
@@ -13201,7 +13464,7 @@
       </c>
       <c r="G27" s="8" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>9.1</v>
+        <v>9.57</v>
       </c>
       <c r="H27" s="6">
         <v>2000</v>
@@ -13216,7 +13479,7 @@
       </c>
       <c r="K27" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>18200</v>
+        <v>19140</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="7"/>
@@ -13253,7 +13516,7 @@
       </c>
       <c r="G28" s="8" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>135.55000000000001</v>
+        <v>157.31</v>
       </c>
       <c r="H28" s="6">
         <v>300</v>
@@ -13268,7 +13531,7 @@
       </c>
       <c r="K28" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>40665</v>
+        <v>47193</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="7"/>
@@ -13305,7 +13568,7 @@
       </c>
       <c r="G29" s="8" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>174.67</v>
+        <v>170.68</v>
       </c>
       <c r="H29" s="6">
         <v>300</v>
@@ -13320,7 +13583,7 @@
       </c>
       <c r="K29" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>52400.999999999993</v>
+        <v>51204</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="7"/>
@@ -13357,7 +13620,7 @@
       </c>
       <c r="G30" s="8" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>325.31</v>
+        <v>327.55</v>
       </c>
       <c r="H30" s="6">
         <v>150</v>
@@ -13372,7 +13635,7 @@
       </c>
       <c r="K30" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>48796.5</v>
+        <v>49132.5</v>
       </c>
       <c r="L30" s="6"/>
       <c r="M30" s="7"/>
@@ -13409,7 +13672,7 @@
       </c>
       <c r="G31" s="8" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>710.85</v>
+        <v>736.3</v>
       </c>
       <c r="H31" s="6">
         <v>100</v>
@@ -13424,7 +13687,7 @@
       </c>
       <c r="K31" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>71085</v>
+        <v>73630</v>
       </c>
       <c r="L31" s="6"/>
       <c r="M31" s="7"/>
@@ -13512,7 +13775,7 @@
       </c>
       <c r="G33" s="8" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H33" s="6">
         <v>63</v>
@@ -13527,7 +13790,7 @@
       </c>
       <c r="K33" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>2618.2800000000002</v>
+        <v>2936.43</v>
       </c>
       <c r="L33" s="6"/>
       <c r="M33" s="7"/>
@@ -13564,7 +13827,7 @@
       </c>
       <c r="G34" s="8" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>137.4</v>
+        <v>142.9</v>
       </c>
       <c r="H34" s="6">
         <v>1500</v>
@@ -13579,7 +13842,7 @@
       </c>
       <c r="K34" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>206100</v>
+        <v>214350</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="7"/>
@@ -13611,7 +13874,7 @@
       </c>
       <c r="G35" s="8" cm="1">
         <f t="array" aca="1" ref="G35" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H35" s="6">
         <v>35</v>
@@ -13626,7 +13889,7 @@
       </c>
       <c r="K35" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>4968.95</v>
+        <v>5400.85</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="7"/>
@@ -13658,7 +13921,7 @@
       </c>
       <c r="G36" s="8" cm="1">
         <f t="array" aca="1" ref="G36" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H36" s="6">
         <v>30</v>
@@ -13673,7 +13936,7 @@
       </c>
       <c r="K36" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>1246.8000000000002</v>
+        <v>1398.3</v>
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="7"/>
@@ -13705,7 +13968,7 @@
       </c>
       <c r="G37" s="8" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H37" s="6">
         <v>30</v>
@@ -13720,7 +13983,7 @@
       </c>
       <c r="K37" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>4259.1000000000004</v>
+        <v>4629.3</v>
       </c>
       <c r="L37" s="6"/>
       <c r="M37" s="7"/>
@@ -13752,7 +14015,7 @@
       </c>
       <c r="G38" s="8" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H38" s="6">
         <v>30</v>
@@ -13767,7 +14030,7 @@
       </c>
       <c r="K38" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>1246.8000000000002</v>
+        <v>1398.3</v>
       </c>
       <c r="L38" s="6"/>
       <c r="M38" s="7"/>
@@ -13799,7 +14062,7 @@
       </c>
       <c r="G39" s="8" cm="1">
         <f t="array" aca="1" ref="G39" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>115.6</v>
+        <v>127.25</v>
       </c>
       <c r="H39" s="6">
         <v>300</v>
@@ -13814,7 +14077,7 @@
       </c>
       <c r="K39" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>34680</v>
+        <v>38175</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="7"/>
@@ -13846,7 +14109,7 @@
       </c>
       <c r="G40" s="8" cm="1">
         <f t="array" aca="1" ref="G40" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>761</v>
+        <v>815.24</v>
       </c>
       <c r="H40" s="6">
         <v>90</v>
@@ -13861,7 +14124,7 @@
       </c>
       <c r="K40" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>68490</v>
+        <v>73371.600000000006</v>
       </c>
       <c r="L40" s="6"/>
       <c r="M40" s="7"/>
@@ -13893,7 +14156,7 @@
       </c>
       <c r="G41" s="8" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>135.55000000000001</v>
+        <v>157.31</v>
       </c>
       <c r="H41" s="6">
         <v>300</v>
@@ -13908,7 +14171,7 @@
       </c>
       <c r="K41" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>40665</v>
+        <v>47193</v>
       </c>
       <c r="L41" s="6"/>
       <c r="M41" s="7"/>
@@ -13940,7 +14203,7 @@
       </c>
       <c r="G42" s="8" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>215.22</v>
+        <v>210.72</v>
       </c>
       <c r="H42" s="6">
         <v>200</v>
@@ -13955,7 +14218,7 @@
       </c>
       <c r="K42" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>43044</v>
+        <v>42144</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="7"/>
@@ -13987,7 +14250,7 @@
       </c>
       <c r="G43" s="8" cm="1">
         <f t="array" aca="1" ref="G43" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>819.36</v>
+        <v>792.3</v>
       </c>
       <c r="H43" s="6">
         <v>40</v>
@@ -14002,12 +14265,12 @@
       </c>
       <c r="K43" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>32774.400000000001</v>
+        <v>31692</v>
       </c>
       <c r="L43" s="6"/>
       <c r="M43" s="7">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Value]]-TableYigaelUSA[[#This Row],[Buy Value]] +TableYigaelUSA[[#This Row],[Dividand]]</f>
-        <v>2494.4000000000015</v>
+        <v>1412</v>
       </c>
       <c r="N43" s="6">
         <f>TableYigaelUSA[[#This Row],[Sell Value]]-TableYigaelUSA[[#This Row],[Buy Value]] +TableYigaelUSA[[#This Row],[Dividand]]</f>
@@ -14037,7 +14300,7 @@
       </c>
       <c r="G44" s="8" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>115.6</v>
+        <v>127.25</v>
       </c>
       <c r="H44" s="6">
         <v>200</v>
@@ -14052,7 +14315,7 @@
       </c>
       <c r="K44" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>23120</v>
+        <v>25450</v>
       </c>
       <c r="L44" s="6"/>
       <c r="M44" s="7"/>
@@ -14084,7 +14347,7 @@
       </c>
       <c r="G45" s="8" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>115.6</v>
+        <v>127.25</v>
       </c>
       <c r="H45" s="6">
         <v>100</v>
@@ -14099,7 +14362,7 @@
       </c>
       <c r="K45" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>11560</v>
+        <v>12725</v>
       </c>
       <c r="L45" s="6"/>
       <c r="M45" s="7"/>
@@ -14131,7 +14394,7 @@
       </c>
       <c r="G46" s="8" cm="1">
         <f t="array" aca="1" ref="G46" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>115.6</v>
+        <v>127.25</v>
       </c>
       <c r="H46" s="6">
         <v>300</v>
@@ -14146,7 +14409,7 @@
       </c>
       <c r="K46" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>34680</v>
+        <v>38175</v>
       </c>
       <c r="L46" s="6"/>
       <c r="M46" s="7"/>
@@ -14178,7 +14441,7 @@
       </c>
       <c r="G47" s="8" cm="1">
         <f t="array" aca="1" ref="G47" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>174.67</v>
+        <v>170.68</v>
       </c>
       <c r="H47" s="6">
         <v>100</v>
@@ -14193,7 +14456,7 @@
       </c>
       <c r="K47" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>17467</v>
+        <v>17068</v>
       </c>
       <c r="L47" s="6"/>
       <c r="M47" s="7"/>
@@ -14225,7 +14488,7 @@
       </c>
       <c r="G48" s="8" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>174.67</v>
+        <v>170.68</v>
       </c>
       <c r="H48" s="6">
         <v>100</v>
@@ -14240,12 +14503,12 @@
       </c>
       <c r="K48" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>17467</v>
+        <v>17068</v>
       </c>
       <c r="L48" s="6"/>
       <c r="M48" s="7">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Value]]-TableYigaelUSA[[#This Row],[Buy Value]] +TableYigaelUSA[[#This Row],[Dividand]]</f>
-        <v>2613.5</v>
+        <v>2214.5</v>
       </c>
       <c r="N48" s="6">
         <f>TableYigaelUSA[[#This Row],[Sell Value]]-TableYigaelUSA[[#This Row],[Buy Value]] +TableYigaelUSA[[#This Row],[Dividand]]</f>
@@ -14275,7 +14538,7 @@
       </c>
       <c r="G49" s="8" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>211.1</v>
+        <v>222.74</v>
       </c>
       <c r="H49" s="6">
         <v>200</v>
@@ -14290,7 +14553,7 @@
       </c>
       <c r="K49" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>42220</v>
+        <v>44548</v>
       </c>
       <c r="L49" s="6"/>
       <c r="M49" s="7"/>
@@ -14322,7 +14585,7 @@
       </c>
       <c r="G50" s="8" cm="1">
         <f t="array" aca="1" ref="G50" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>116.16</v>
+        <v>143.4</v>
       </c>
       <c r="H50" s="6">
         <v>650</v>
@@ -14337,7 +14600,7 @@
       </c>
       <c r="K50" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>75504</v>
+        <v>93210</v>
       </c>
       <c r="L50" s="6"/>
       <c r="M50" s="7"/>
@@ -14369,7 +14632,7 @@
       </c>
       <c r="G51" s="8" cm="1">
         <f t="array" aca="1" ref="G51" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H51" s="6">
         <v>60</v>
@@ -14384,7 +14647,7 @@
       </c>
       <c r="K51" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>2493.6000000000004</v>
+        <v>2796.6</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="7"/>
@@ -14416,7 +14679,7 @@
       </c>
       <c r="G52" s="8" cm="1">
         <f t="array" aca="1" ref="G52" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>141.97</v>
+        <v>154.31</v>
       </c>
       <c r="H52" s="6">
         <v>60</v>
@@ -14431,7 +14694,7 @@
       </c>
       <c r="K52" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>8518.2000000000007</v>
+        <v>9258.6</v>
       </c>
       <c r="L52" s="6"/>
       <c r="M52" s="7"/>
@@ -14506,7 +14769,7 @@
       </c>
       <c r="G54" s="8" cm="1">
         <f t="array" aca="1" ref="G54" ca="1">_FV(TableYigaelUSA[[#This Row],[Instrumant]],"Price")</f>
-        <v>41.56</v>
+        <v>46.61</v>
       </c>
       <c r="H54" s="6">
         <v>200</v>
@@ -14521,7 +14784,7 @@
       </c>
       <c r="K54" s="8">
         <f ca="1">TableYigaelUSA[[#This Row],[Current Price]]*TableYigaelUSA[[#This Row],[Order ammount]]</f>
-        <v>8312</v>
+        <v>9322</v>
       </c>
       <c r="L54" s="6"/>
       <c r="M54" s="7"/>
@@ -14690,7 +14953,7 @@
       </c>
       <c r="B7">
         <f ca="1">Realized_and_Unrealized_Profit_Yigael_USA*USD_ILS_Price</f>
-        <v>96609.116981393978</v>
+        <v>92536.174033163974</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>